<commit_message>
Se actualiza la descripcion del proyecto.
</commit_message>
<xml_diff>
--- a/Programas/estructura paso.xlsx
+++ b/Programas/estructura paso.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="211"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="78">
   <si>
     <t>Paso</t>
   </si>
@@ -229,6 +229,27 @@
   </si>
   <si>
     <t>gradiente(°C/min)</t>
+  </si>
+  <si>
+    <t>ROTACION</t>
+  </si>
+  <si>
+    <t>LLENADO</t>
+  </si>
+  <si>
+    <t>DESAGUE</t>
+  </si>
+  <si>
+    <t>ADITIVOS</t>
+  </si>
+  <si>
+    <t>MUESTREO</t>
+  </si>
+  <si>
+    <t>TEMPERATURA</t>
+  </si>
+  <si>
+    <t>MANTENIMIENTO</t>
   </si>
 </sst>
 </file>
@@ -312,19 +333,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -410,7 +431,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -702,28 +723,28 @@
   <dimension ref="A2:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="10" width="16.5703125" customWidth="1"/>
     <col min="11" max="1023" width="11.5703125"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
     </row>
     <row r="3" spans="1:10" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
@@ -782,21 +803,23 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7">
         <v>1</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
+      <c r="A6" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="B6" s="2">
         <v>2</v>
       </c>
@@ -814,25 +837,29 @@
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11">
+      <c r="A7" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="7">
         <v>3</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11" t="s">
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="I7" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="J7" s="11"/>
+      <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
+      <c r="A8" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B8" s="2">
         <v>4</v>
       </c>
@@ -848,23 +875,27 @@
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:10" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11">
+      <c r="A9" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="7">
         <v>5</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11" t="s">
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="J9" s="11"/>
+      <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
+      <c r="A10" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="B10" s="2">
         <v>6</v>
       </c>
@@ -878,21 +909,25 @@
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:10" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11">
+      <c r="A11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="7">
         <v>7</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
     </row>
     <row r="12" spans="1:10" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
+      <c r="A12" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="B12" s="2">
         <v>8</v>
       </c>
@@ -910,22 +945,24 @@
       <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:10" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11">
+      <c r="A13" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" s="7">
         <v>9</v>
       </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11" t="s">
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="I13" s="11" t="s">
+      <c r="I13" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="J13" s="11"/>
+      <c r="J13" s="7"/>
     </row>
     <row r="14" spans="1:10" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
@@ -964,20 +1001,20 @@
       <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:10" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="9" t="s">
+      <c r="G17" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
     </row>
     <row r="18" spans="1:10" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
@@ -1223,11 +1260,11 @@
       <c r="A28" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="2" t="s">
@@ -1248,11 +1285,11 @@
       <c r="A29" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="2"/>
@@ -1267,11 +1304,11 @@
       <c r="A30" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="2"/>
@@ -1286,9 +1323,9 @@
       <c r="A31" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
@@ -1300,11 +1337,11 @@
       <c r="A32" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
@@ -1316,11 +1353,11 @@
       <c r="A33" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
@@ -1330,11 +1367,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="G17:J17"/>
     <mergeCell ref="B31:D31"/>
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="B33:D33"/>
@@ -1343,12 +1381,11 @@
     <mergeCell ref="B28:D28"/>
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="B30:D30"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="landscape" useFirstPageNumber="1" r:id="rId1"/>
@@ -1367,7 +1404,7 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1025" width="11.5703125"/>
   </cols>
@@ -1465,7 +1502,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1025" width="11.5703125"/>
   </cols>

</xml_diff>